<commit_message>
General Description: Changed Stats.xlsx and added function to add berry-vil. 1) In Stats.xlsx the effect AoESim.State.MaxPop = AoESim.State.MaxPop + AoESim.Consts.PopPerHouse; for the house was still there    but it should have read AoESim.CurState.MaxPop = AoESim.CurState.MaxPop + AoESim.Consts.PopPerHouse; 2) Added function BuildBerryVil which adds a villager to berries. Should it automatically build a mill if possible and available?
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Buildings" sheetId="1" state="visible" r:id="rId2"/>
@@ -87,7 +87,7 @@
     <t xml:space="preserve">House</t>
   </si>
   <si>
-    <t xml:space="preserve">AoESim.State.MaxPop = AoESim.State.MaxPop + AoESim.Consts.PopPerHouse;</t>
+    <t xml:space="preserve">AoESim.CurState.MaxPop = AoESim.CurState.MaxPop + AoESim.Consts.PopPerHouse;</t>
   </si>
   <si>
     <t xml:space="preserve">Lumber Camp</t>
@@ -1136,11 +1136,11 @@
   </sheetPr>
   <dimension ref="A1:W327"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.71"/>
@@ -2171,7 +2171,7 @@
       <selection pane="topLeft" activeCell="J131" activeCellId="0" sqref="J131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.46"/>
@@ -6580,11 +6580,11 @@
   </sheetPr>
   <dimension ref="A1:J137"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.88"/>

</xml_diff>